<commit_message>
Luke Dysart final push
</commit_message>
<xml_diff>
--- a/scripts/SBOL_xlsx5.xlsx
+++ b/scripts/SBOL_xlsx5.xlsx
@@ -49,19 +49,19 @@
     <t>A5</t>
   </si>
   <si>
+    <t>https://sbolcanvas.org/B0034/1</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>https://sbolcanvas.org/B0015/1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
     <t>https://sbolcanvas.org/GFP/1</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>https://sbolcanvas.org/B0034/1</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>https://sbolcanvas.org/B0015/1</t>
   </si>
   <si>
     <t>B2</t>

</xml_diff>